<commit_message>
Added email and pdf report
</commit_message>
<xml_diff>
--- a/SmokeTestData.xlsx
+++ b/SmokeTestData.xlsx
@@ -1,36 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Qiao\AA Enhanced\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumar\Downloads\AA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30C287A-48C4-4256-8A04-40E57B200D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11295" tabRatio="990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="3" r:id="rId1"/>
-    <sheet name="Library" sheetId="10" r:id="rId2"/>
-    <sheet name="BillingContact" sheetId="11" r:id="rId3"/>
-    <sheet name="BillingTE" sheetId="13" r:id="rId4"/>
-    <sheet name="Bill" sheetId="14" r:id="rId5"/>
-    <sheet name="BillingFile" sheetId="12" r:id="rId6"/>
-    <sheet name="TimeSheets" sheetId="8" r:id="rId7"/>
-    <sheet name="Documents" sheetId="9" r:id="rId8"/>
-    <sheet name="Contact" sheetId="1" r:id="rId9"/>
-    <sheet name="PrecedentFile" sheetId="17" r:id="rId10"/>
-    <sheet name="ContactAPX" sheetId="15" r:id="rId11"/>
-    <sheet name="File" sheetId="2" r:id="rId12"/>
-    <sheet name="FileAPX" sheetId="16" r:id="rId13"/>
-    <sheet name="Calendar" sheetId="4" r:id="rId14"/>
-    <sheet name="Note" sheetId="5" r:id="rId15"/>
-    <sheet name="Tasks" sheetId="6" r:id="rId16"/>
-    <sheet name="PhoneCalls" sheetId="7" r:id="rId17"/>
+    <sheet name="SendEmail" sheetId="18" r:id="rId2"/>
+    <sheet name="ReportPDF" sheetId="19" r:id="rId3"/>
+    <sheet name="Library" sheetId="10" r:id="rId4"/>
+    <sheet name="BillingContact" sheetId="11" r:id="rId5"/>
+    <sheet name="BillingTE" sheetId="13" r:id="rId6"/>
+    <sheet name="Bill" sheetId="14" r:id="rId7"/>
+    <sheet name="BillingFile" sheetId="12" r:id="rId8"/>
+    <sheet name="TimeSheets" sheetId="8" r:id="rId9"/>
+    <sheet name="Documents" sheetId="9" r:id="rId10"/>
+    <sheet name="Contact" sheetId="1" r:id="rId11"/>
+    <sheet name="PrecedentFile" sheetId="17" r:id="rId12"/>
+    <sheet name="ContactAPX" sheetId="15" r:id="rId13"/>
+    <sheet name="File" sheetId="2" r:id="rId14"/>
+    <sheet name="FileAPX" sheetId="16" r:id="rId15"/>
+    <sheet name="Calendar" sheetId="4" r:id="rId16"/>
+    <sheet name="Note" sheetId="5" r:id="rId17"/>
+    <sheet name="Tasks" sheetId="6" r:id="rId18"/>
+    <sheet name="PhoneCalls" sheetId="7" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="122">
   <si>
     <t>FirstName</t>
   </si>
@@ -344,15 +347,92 @@
   <si>
     <t>Automation</t>
   </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>ServerHostName</t>
+  </si>
+  <si>
+    <t>ServerPort</t>
+  </si>
+  <si>
+    <t>UseSSL</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>SendEmailOnFailure</t>
+  </si>
+  <si>
+    <t>SendEmailOnSuccess</t>
+  </si>
+  <si>
+    <t>SendZippedReportOnComplete</t>
+  </si>
+  <si>
+    <t>PDFReportCustomStyleSheet</t>
+  </si>
+  <si>
+    <t>Build AA Automation 2019</t>
+  </si>
+  <si>
+    <t>mmargasagayam@abacusnext.com</t>
+  </si>
+  <si>
+    <t>amicustestmk1@gmail.com</t>
+  </si>
+  <si>
+    <t>smtp.gmail.com</t>
+  </si>
+  <si>
+    <t>0nXTeam123$$</t>
+  </si>
+  <si>
+    <t>SendPDFReportOnComplete</t>
+  </si>
+  <si>
+    <t>PdfName</t>
+  </si>
+  <si>
+    <t>PdfDirectoryPath</t>
+  </si>
+  <si>
+    <t>Xml</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>DeleteRanorexReport</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,10 +455,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -418,8 +499,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -697,11 +780,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +828,132 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="24.28515625" style="3"/>
+    <col min="3" max="3" width="22.85546875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="24.28515625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -786,8 +994,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -875,8 +1083,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -917,8 +1125,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -959,8 +1167,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1028,11 +1236,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">TEXT(NOW(), "hh:mm AM/PM")</f>
-        <v>06:09 PM</v>
+        <v>02:08 PM</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">TEXT(NOW()+1/24, "hh:mm AM/PM")</f>
-        <v>07:09 PM</v>
+        <v>03:08 PM</v>
       </c>
       <c r="H2" t="s">
         <v>26</v>
@@ -1050,8 +1258,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1099,8 +1307,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1140,8 +1348,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1183,7 +1391,165 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A18FE9B-22A0-47EF-B027-8790BDE933CA}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2">
+        <v>587</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E3AE2A92-9EDF-4917-A743-0B484E9C339E}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{12E337A2-5DDD-4AAD-BE98-C27444EF99EE}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{4F8B4FA5-D81A-468A-98D2-17A2E3A312CD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65CC738-6838-47A1-86AC-005575AEA6D1}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1232,8 +1598,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1303,8 +1669,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1373,8 +1739,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1515,8 +1881,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1557,8 +1923,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1598,129 +1964,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="24.28515625" style="3"/>
-    <col min="3" max="3" width="22.85546875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="24.28515625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added from automation box ads 5087, changes to email module
</commit_message>
<xml_diff>
--- a/SmokeTestData.xlsx
+++ b/SmokeTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20346"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumar\Downloads\AA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qa\Downloads\AA_updated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30C287A-48C4-4256-8A04-40E57B200D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4361E1D5-7E0D-4ED6-9690-3AC246A167DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,17 +33,11 @@
     <sheet name="Tasks" sheetId="6" r:id="rId18"/>
     <sheet name="PhoneCalls" sheetId="7" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -387,9 +381,6 @@
     <t>Build AA Automation 2019</t>
   </si>
   <si>
-    <t>mmargasagayam@abacusnext.com</t>
-  </si>
-  <si>
     <t>amicustestmk1@gmail.com</t>
   </si>
   <si>
@@ -415,6 +406,9 @@
   </si>
   <si>
     <t>DeleteRanorexReport</t>
+  </si>
+  <si>
+    <t>mmargasagayam@abacusnext.com;dgopakumar@abacusnext.com;dumendoza@abacusnext.com;Kumar@abacusnext.com;dwolfendale@abacusnext.com</t>
   </si>
 </sst>
 </file>
@@ -459,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -499,7 +493,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1236,11 +1231,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">TEXT(NOW(), "hh:mm AM/PM")</f>
-        <v>02:08 PM</v>
+        <v>02:39 PM</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">TEXT(NOW()+1/24, "hh:mm AM/PM")</f>
-        <v>03:08 PM</v>
+        <v>03:39 PM</v>
       </c>
       <c r="H2" t="s">
         <v>26</v>
@@ -1395,14 +1390,14 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="81" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1454,7 +1449,7 @@
         <v>109</v>
       </c>
       <c r="M1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N1" t="s">
         <v>110</v>
@@ -1465,14 +1460,14 @@
         <v>111</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" t="s">
         <v>113</v>
-      </c>
-      <c r="E2" t="s">
-        <v>114</v>
       </c>
       <c r="F2">
         <v>587</v>
@@ -1481,10 +1476,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -1501,9 +1496,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{E3AE2A92-9EDF-4917-A743-0B484E9C339E}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{12E337A2-5DDD-4AAD-BE98-C27444EF99EE}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{4F8B4FA5-D81A-468A-98D2-17A2E3A312CD}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{01352938-D531-4433-B256-64BD0B127D1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1528,19 +1521,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
         <v>117</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>118</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>119</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>120</v>
-      </c>
-      <c r="E1" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Login Module and Word Add In
</commit_message>
<xml_diff>
--- a/SmokeTestData.xlsx
+++ b/SmokeTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumar\Downloads\AA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qa\Downloads\AA_updated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90ECEDB-5F44-4537-8F09-F6A120D6F05B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAB30F0-E540-4C02-8536-BEF5ED3896B5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,16 +405,16 @@
     <t>mmargasagayam@abacusnext.com;dgopakumar@abacusnext.com;dumendoza@abacusnext.com;Kumar@abacusnext.com;dwolfendale@abacusnext.com</t>
   </si>
   <si>
-    <t>QA Toronto 10</t>
-  </si>
-  <si>
-    <t>Admin User</t>
-  </si>
-  <si>
-    <t>Mohan Kumar</t>
-  </si>
-  <si>
-    <t>J4-Mohanss</t>
+    <t>firmid</t>
+  </si>
+  <si>
+    <t>QA User1</t>
+  </si>
+  <si>
+    <t>newautomation</t>
+  </si>
+  <si>
+    <t>Amicus User</t>
   </si>
 </sst>
 </file>
@@ -785,7 +785,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,13 +815,13 @@
         <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1252,11 +1252,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">TEXT(NOW(), "hh:mm AM/PM")</f>
-        <v>02:02 PM</v>
+        <v>05:34 PM</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">TEXT(NOW()+1/24, "hh:mm AM/PM")</f>
-        <v>03:02 PM</v>
+        <v>06:34 PM</v>
       </c>
       <c r="H2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Added Billing Trust and Time entry Fees Expenses
</commit_message>
<xml_diff>
--- a/SmokeTestData.xlsx
+++ b/SmokeTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qa\Downloads\AA_updated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumar\Downloads\AA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAB30F0-E540-4C02-8536-BEF5ED3896B5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB594287-9182-4773-B4D5-EC2726180AB9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="125">
   <si>
     <t>FirstName</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>Amicus User</t>
+  </si>
+  <si>
+    <t>Mohan Kumar</t>
   </si>
 </sst>
 </file>
@@ -782,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,6 +838,20 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1252,11 +1269,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">TEXT(NOW(), "hh:mm AM/PM")</f>
-        <v>05:34 PM</v>
+        <v>11:43 AM</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">TEXT(NOW()+1/24, "hh:mm AM/PM")</f>
-        <v>06:34 PM</v>
+        <v>12:43 PM</v>
       </c>
       <c r="H2" t="s">
         <v>26</v>

</xml_diff>